<commit_message>
Liga Femenina añadida con exito 100%
</commit_message>
<xml_diff>
--- a/Output Primera Division.xlsx
+++ b/Output Primera Division.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="120">
   <si>
     <t>Team</t>
   </si>
@@ -215,76 +215,79 @@
     <t>56</t>
   </si>
   <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>45</t>
+    <t>51</t>
+  </si>
+  <si>
+    <t>43</t>
   </si>
   <si>
     <t>38</t>
   </si>
   <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>43</t>
+    <t>40</t>
   </si>
   <si>
     <t>44</t>
   </si>
   <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>['Girona', 'Real Betis', 'Sevilla', 'Villarreal']</t>
   </si>
   <si>
-    <t>['Valencia', 'Elche']</t>
-  </si>
-  <si>
-    <t>['Espanyol', 'Celta']</t>
+    <t>['Valencia', 'Elche', 'Osasuna']</t>
+  </si>
+  <si>
+    <t>['Espanyol']</t>
   </si>
   <si>
     <t>['Real Valladolid', 'Osasuna', 'Celta']</t>
   </si>
   <si>
-    <t>['Getafe', 'AlmerÃ\xada']</t>
+    <t>['AlmerÃ\xada', 'Real Valladolid']</t>
   </si>
   <si>
     <t>['Villarreal', 'AlmerÃ\xada']</t>
@@ -293,30 +296,24 @@
     <t>['CÃ¡diz', 'Valencia']</t>
   </si>
   <si>
-    <t>['Girona']</t>
+    <t>['Real Madrid', 'Villarreal']</t>
   </si>
   <si>
     <t>[]</t>
   </si>
   <si>
-    <t>['Celta', 'Real Madrid']</t>
-  </si>
-  <si>
     <t>['Valencia', 'AlmerÃ\xada']</t>
   </si>
   <si>
     <t>['CÃ¡diz', 'Elche', 'Mallorca']</t>
   </si>
   <si>
+    <t>['Athletic', 'Real Betis']</t>
+  </si>
+  <si>
     <t>['Valencia', 'R. Sociedad']</t>
   </si>
   <si>
-    <t>['Athletic', 'Real Betis']</t>
-  </si>
-  <si>
-    <t>['Espanyol']</t>
-  </si>
-  <si>
     <t>['Mallorca', 'Girona']</t>
   </si>
   <si>
@@ -341,24 +338,24 @@
     <t>['Real Madrid', 'Celta']</t>
   </si>
   <si>
-    <t>['Rayo Vallecano', 'Elche', 'Barcelona']</t>
+    <t>['CÃ¡diz', 'Sevilla']</t>
+  </si>
+  <si>
+    <t>['Rayo Vallecano', 'Elche', 'Barcelona', 'Mallorca']</t>
+  </si>
+  <si>
+    <t>['AtlÃ©tico', 'Real Madrid']</t>
+  </si>
+  <si>
+    <t>['Barcelona', 'CÃ¡diz']</t>
+  </si>
+  <si>
+    <t>['Barcelona']</t>
   </si>
   <si>
     <t>['AtlÃ©tico']</t>
   </si>
   <si>
-    <t>['CÃ¡diz', 'Sevilla']</t>
-  </si>
-  <si>
-    <t>['Barcelona', 'CÃ¡diz']</t>
-  </si>
-  <si>
-    <t>['Barcelona']</t>
-  </si>
-  <si>
-    <t>['AtlÃ©tico', 'R. Sociedad']</t>
-  </si>
-  <si>
     <t>['Rayo Vallecano', 'Real Betis', 'Girona']</t>
   </si>
   <si>
@@ -377,13 +374,10 @@
     <t>['Sevilla', 'Real Madrid']</t>
   </si>
   <si>
-    <t>['Real Madrid']</t>
-  </si>
-  <si>
     <t>['Getafe']</t>
   </si>
   <si>
-    <t>['Elche', 'Espanyol', 'Real Valladolid']</t>
+    <t>['Espanyol', 'Real Valladolid']</t>
   </si>
   <si>
     <t>['Osasuna']</t>
@@ -554,10 +548,10 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -646,10 +640,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -830,7 +824,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,7 +1160,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1270,13 +1264,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -1285,7 +1279,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17</c:v>
@@ -1300,7 +1294,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
@@ -1318,16 +1312,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,16 +1422,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
@@ -1446,7 +1440,7 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1461,7 +1455,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3</c:v>
@@ -1479,13 +1473,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.75</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1640,7 +1634,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1744,13 +1738,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4</c:v>
@@ -1759,10 +1753,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1774,10 +1768,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3</c:v>
@@ -1789,19 +1783,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1959,7 +1953,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2114,10 +2108,10 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2221,7 +2215,7 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>9</c:v>
@@ -2230,14 +2224,14 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>18</c:v>
-                </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2248,34 +2242,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.5</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.25</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2376,25 +2370,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2406,34 +2400,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.5</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.75</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2534,25 +2528,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2564,7 +2558,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>4</c:v>
@@ -2582,16 +2576,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.5</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2746,10 +2740,10 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2904,7 +2898,7 @@
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1</c:v>
@@ -3011,22 +3005,22 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3038,13 +3032,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -3056,13 +3050,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.75</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1</c:v>
@@ -3166,25 +3160,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3196,31 +3190,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.25</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>4</c:v>
@@ -3378,10 +3372,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3536,10 +3530,10 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3694,10 +3688,10 @@
                   <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4013,7 +4007,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4168,10 +4162,10 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4328,7 +4322,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -4346,13 +4340,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.75</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4417,7 +4411,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -4435,16 +4429,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.25</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4598,10 +4592,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -4613,19 +4607,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4690,10 +4684,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -4702,22 +4696,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.75</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>22</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4871,13 +4865,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -4889,16 +4883,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4963,34 +4957,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.25</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5144,10 +5138,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -5156,22 +5150,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.75</c:v>
-                </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5236,7 +5230,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -5254,16 +5248,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5441,10 +5435,10 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5533,10 +5527,10 @@
                   <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5717,7 +5711,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5806,7 +5800,7 @@
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -5987,7 +5981,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -6079,10 +6073,10 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6260,7 +6254,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -6352,10 +6346,10 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7184,10 +7178,10 @@
         <v>1.25</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K2">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -7219,10 +7213,10 @@
         <v>3</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K3">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -7309,7 +7303,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -7443,7 +7437,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
         <v>59</v>
@@ -7455,19 +7449,19 @@
         <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
         <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M2">
         <v>7</v>
@@ -7494,7 +7488,7 @@
         <v>0.25</v>
       </c>
       <c r="U2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -7511,10 +7505,10 @@
         <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
@@ -7523,22 +7517,22 @@
         <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I3" t="s">
         <v>58</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="M3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -7556,16 +7550,16 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="T3">
         <v>0.25</v>
       </c>
       <c r="U3">
+        <v>4</v>
+      </c>
+      <c r="V3">
         <v>10</v>
-      </c>
-      <c r="V3">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -7579,13 +7573,13 @@
         <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
         <v>46</v>
@@ -7594,22 +7588,22 @@
         <v>68</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L4" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="M4">
         <v>4</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O4">
         <v>3</v>
@@ -7627,13 +7621,13 @@
         <v>1</v>
       </c>
       <c r="T4">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -7647,7 +7641,7 @@
         <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
         <v>52</v>
@@ -7665,13 +7659,13 @@
         <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M5">
         <v>6</v>
@@ -7698,7 +7692,7 @@
         <v>0.25</v>
       </c>
       <c r="U5">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -7715,10 +7709,10 @@
         <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -7727,25 +7721,25 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O6">
         <v>3</v>
@@ -7757,19 +7751,19 @@
         <v>4</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="T6">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="U6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="V6">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -7783,7 +7777,7 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
         <v>50</v>
@@ -7795,19 +7789,19 @@
         <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M7">
         <v>4</v>
@@ -7837,7 +7831,7 @@
         <v>9</v>
       </c>
       <c r="V7">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -7851,7 +7845,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
         <v>50</v>
@@ -7866,16 +7860,16 @@
         <v>69</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -7902,10 +7896,10 @@
         <v>1.25</v>
       </c>
       <c r="U8">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V8">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -7913,13 +7907,13 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
         <v>50</v>
@@ -7928,52 +7922,52 @@
         <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="T9">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="U9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V9">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -7981,67 +7975,67 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="J10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L10" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>9</v>
+      </c>
+      <c r="O10">
         <v>2</v>
-      </c>
-      <c r="N10">
-        <v>3</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
+        <v>4</v>
+      </c>
+      <c r="R10">
         <v>1</v>
       </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
       <c r="S10">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="T10">
-        <v>0.75</v>
+        <v>2.25</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -8049,40 +8043,40 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
         <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
         <v>91</v>
       </c>
       <c r="K11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L11" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <v>4</v>
@@ -8100,16 +8094,16 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="T11">
         <v>1</v>
       </c>
       <c r="U11">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -8120,10 +8114,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
         <v>48</v>
@@ -8144,10 +8138,10 @@
         <v>92</v>
       </c>
       <c r="K12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M12">
         <v>7</v>
@@ -8174,10 +8168,10 @@
         <v>1.25</v>
       </c>
       <c r="U12">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="V12">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -8188,10 +8182,10 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
@@ -8203,19 +8197,19 @@
         <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J13" t="s">
         <v>93</v>
       </c>
       <c r="K13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M13">
         <v>6</v>
@@ -8242,7 +8236,7 @@
         <v>0.75</v>
       </c>
       <c r="U13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V13">
         <v>1</v>
@@ -8253,46 +8247,46 @@
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
         <v>73</v>
       </c>
-      <c r="D14" t="s">
-        <v>76</v>
-      </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="J14" t="s">
         <v>94</v>
       </c>
       <c r="K14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="L14" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="M14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -8304,13 +8298,13 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="T14">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="U14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V14">
         <v>1</v>
@@ -8321,64 +8315,64 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J15" t="s">
         <v>95</v>
       </c>
       <c r="K15" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="L15" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="M15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="T15">
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
       <c r="U15">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="V15">
         <v>4</v>
@@ -8392,10 +8386,10 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
@@ -8407,19 +8401,19 @@
         <v>53</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I16" t="s">
         <v>81</v>
       </c>
       <c r="J16" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="K16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M16">
         <v>7</v>
@@ -8446,10 +8440,10 @@
         <v>3</v>
       </c>
       <c r="U16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="V16">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -8460,10 +8454,10 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
@@ -8481,13 +8475,13 @@
         <v>67</v>
       </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M17">
         <v>5</v>
@@ -8514,10 +8508,10 @@
         <v>1.25</v>
       </c>
       <c r="U17">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="V17">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:22">
@@ -8528,10 +8522,10 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
         <v>45</v>
@@ -8549,13 +8543,13 @@
         <v>67</v>
       </c>
       <c r="J18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M18">
         <v>5</v>
@@ -8582,10 +8576,10 @@
         <v>1.75</v>
       </c>
       <c r="U18">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="V18">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:22">
@@ -8599,7 +8593,7 @@
         <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
         <v>46</v>
@@ -8617,13 +8611,13 @@
         <v>79</v>
       </c>
       <c r="J19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -8667,7 +8661,7 @@
         <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
         <v>45</v>
@@ -8682,16 +8676,16 @@
         <v>59</v>
       </c>
       <c r="I20" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="J20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M20">
         <v>2</v>
@@ -8721,7 +8715,7 @@
         <v>0</v>
       </c>
       <c r="V20">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:22">
@@ -8735,7 +8729,7 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
         <v>42</v>
@@ -8750,16 +8744,16 @@
         <v>56</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M21">
         <v>4</v>
@@ -8786,10 +8780,10 @@
         <v>2.25</v>
       </c>
       <c r="U21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="V21">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -8852,7 +8846,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -8870,13 +8864,13 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -8884,7 +8878,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -8902,16 +8896,16 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="I3">
         <v>1.25</v>
       </c>
       <c r="J3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8971,10 +8965,10 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -8986,19 +8980,19 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -9006,10 +9000,10 @@
         <v>16</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -9018,22 +9012,22 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
+        <v>0.75</v>
+      </c>
+      <c r="I3">
         <v>0.5</v>
       </c>
-      <c r="I3">
-        <v>0.75</v>
-      </c>
       <c r="J3">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -9093,13 +9087,13 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -9111,16 +9105,16 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="K2">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -9128,34 +9122,34 @@
         <v>18</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>2</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.75</v>
+      </c>
+      <c r="I3">
+        <v>2.25</v>
+      </c>
+      <c r="J3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>0.5</v>
-      </c>
-      <c r="I3">
-        <v>1.25</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
       <c r="K3">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -9215,10 +9209,10 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -9227,22 +9221,22 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="I2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -9250,7 +9244,7 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -9268,16 +9262,16 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>0.25</v>
       </c>
       <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
         <v>10</v>
-      </c>
-      <c r="K3">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -9361,10 +9355,10 @@
         <v>2.25</v>
       </c>
       <c r="J2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -9396,10 +9390,10 @@
         <v>1.75</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K3">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -9486,7 +9480,7 @@
         <v>9</v>
       </c>
       <c r="K2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -9518,7 +9512,7 @@
         <v>0.75</v>
       </c>
       <c r="J3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -9605,7 +9599,7 @@
         <v>0.25</v>
       </c>
       <c r="J2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -9640,10 +9634,10 @@
         <v>1.25</v>
       </c>
       <c r="J3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -9727,7 +9721,7 @@
         <v>0.25</v>
       </c>
       <c r="J2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -9762,10 +9756,10 @@
         <v>1.25</v>
       </c>
       <c r="J3">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Back up 1 adding %
</commit_message>
<xml_diff>
--- a/Output Primera Division.xlsx
+++ b/Output Primera Division.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\Desktop\Projects\Python Programs\Bets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782BE498-E379-48CC-AD2B-9DBBE647F207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5D2EB6-D2A8-461D-8899-4ECA5CE21EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="2385" windowWidth="21600" windowHeight="11385" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6615" yWindow="1230" windowWidth="21600" windowHeight="11385" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elche vs Real Betis" sheetId="1" r:id="rId1"/>
@@ -459,12 +459,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -494,12 +500,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7153,15 +7160,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>1228725</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8084,8 +8091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8639,139 +8646,139 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="3">
         <v>6</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="3">
         <v>6</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="3">
         <v>4</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="3">
         <v>0</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="3">
         <v>2</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="3">
         <v>0</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="3">
         <v>1.2</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="3">
         <v>1.2</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="3">
         <v>32</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="3">
         <v>4</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="3">
         <v>9</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="3">
         <v>2</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="3">
         <v>0</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="3">
         <v>4</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="3">
         <v>0</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="3">
         <v>0.8</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="3">
         <v>1.8</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="3">
         <v>18</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="3">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FactorDegenerativo Added to each journey
</commit_message>
<xml_diff>
--- a/Output Primera Division.xlsx
+++ b/Output Primera Division.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\Desktop\Projects\Python Programs\Bets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5D2EB6-D2A8-461D-8899-4ECA5CE21EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="1230" windowWidth="21600" windowHeight="11385" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Elche vs Real Betis" sheetId="1" r:id="rId1"/>
@@ -25,25 +19,12 @@
     <sheet name="Villarreal vs Getafe" sheetId="10" r:id="rId10"/>
     <sheet name="Data Raw Primera" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="129">
   <si>
     <t>Team</t>
   </si>
@@ -430,19 +411,13 @@
   </si>
   <si>
     <t>['AtlÃ©tico', 'Rayo Vallecano']</t>
-  </si>
-  <si>
-    <t>cadiz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rayo </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,18 +434,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -500,51 +469,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -559,7 +506,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Elche vs Real Betis'!$B$1:$K$1</c:f>
@@ -637,11 +583,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FE7A-4DE8-ABC1-94768042705A}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -657,7 +598,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Elche vs Real Betis'!$B$1:$K$1</c:f>
@@ -735,20 +675,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FE7A-4DE8-ABC1-94768042705A}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
@@ -758,7 +685,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -776,25 +702,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -812,11 +733,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
@@ -825,11 +744,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -840,26 +757,14 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -874,7 +779,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Villarreal vs Getafe'!$B$1:$K$1</c:f>
@@ -952,11 +856,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CAC7-4FB7-B2A3-189BCDA7664F}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -972,7 +871,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Villarreal vs Getafe'!$B$1:$K$1</c:f>
@@ -1050,20 +948,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CAC7-4FB7-B2A3-189BCDA7664F}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50100001"/>
         <c:axId val="50100002"/>
@@ -1073,7 +958,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1091,25 +975,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50100002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50100002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1127,11 +1006,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50100001"/>
         <c:crosses val="autoZero"/>
@@ -1140,11 +1017,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1155,26 +1030,14 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1189,7 +1052,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1271,25 +1133,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1333,11 +1195,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1353,7 +1210,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1435,25 +1291,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1497,11 +1353,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1517,7 +1368,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1599,25 +1449,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1661,11 +1511,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1681,7 +1526,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1763,25 +1607,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1825,11 +1669,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1845,7 +1684,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1927,25 +1765,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1989,11 +1827,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -2009,7 +1842,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2091,25 +1923,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2153,11 +1985,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -2173,7 +2000,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2255,25 +2081,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2317,11 +2143,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -2337,7 +2158,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2419,25 +2239,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2481,11 +2301,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
@@ -2501,7 +2316,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2583,25 +2397,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2645,11 +2459,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
@@ -2665,7 +2474,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2747,25 +2555,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2809,11 +2617,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
@@ -2829,7 +2632,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2911,25 +2713,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2973,11 +2775,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
@@ -2993,7 +2790,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3075,25 +2871,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3137,11 +2933,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="12"/>
@@ -3157,7 +2948,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3239,25 +3029,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3301,11 +3091,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="13"/>
@@ -3321,7 +3106,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3403,25 +3187,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3465,11 +3249,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="14"/>
@@ -3485,7 +3264,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3567,25 +3345,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3629,11 +3407,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="15"/>
@@ -3649,7 +3422,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3731,25 +3503,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3793,11 +3565,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="16"/>
@@ -3813,7 +3580,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3895,25 +3661,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3957,11 +3723,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="17"/>
@@ -3977,7 +3738,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -4059,25 +3819,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4121,11 +3881,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000011-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="18"/>
@@ -4141,7 +3896,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -4223,25 +3977,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4285,11 +4039,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="19"/>
@@ -4305,7 +4054,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -4387,25 +4135,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4449,20 +4197,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000013-E5A6-416F-91A3-3FC3777A0E0D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50110001"/>
         <c:axId val="50110002"/>
@@ -4472,7 +4207,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4490,25 +4224,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50110002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50110002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -4526,11 +4255,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50110001"/>
         <c:crosses val="autoZero"/>
@@ -4539,11 +4266,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4554,26 +4279,14 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4588,7 +4301,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Espanyol vs Mallorca'!$B$1:$K$1</c:f>
@@ -4666,11 +4378,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C649-4362-A700-25D3B10546F4}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4686,7 +4393,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Espanyol vs Mallorca'!$B$1:$K$1</c:f>
@@ -4764,20 +4470,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C649-4362-A700-25D3B10546F4}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50020001"/>
         <c:axId val="50020002"/>
@@ -4787,7 +4480,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4805,25 +4497,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50020002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -4841,11 +4528,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
@@ -4854,11 +4539,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4869,26 +4552,14 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4903,7 +4574,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'CÃ¡diz vs Rayo Vallecano'!$B$1:$K$1</c:f>
@@ -4981,11 +4651,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-042D-4120-AD9E-14DCC44F0AC8}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5001,7 +4666,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'CÃ¡diz vs Rayo Vallecano'!$B$1:$K$1</c:f>
@@ -5079,20 +4743,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-042D-4120-AD9E-14DCC44F0AC8}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50030001"/>
         <c:axId val="50030002"/>
@@ -5102,7 +4753,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5120,25 +4770,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50030002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5156,11 +4801,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030001"/>
         <c:crosses val="autoZero"/>
@@ -5169,11 +4812,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5184,26 +4825,14 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5218,7 +4847,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Real Madrid vs AtlÃ©tico'!$B$1:$K$1</c:f>
@@ -5296,11 +4924,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AD24-4FB8-B210-037E9C2A0669}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5316,7 +4939,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Real Madrid vs AtlÃ©tico'!$B$1:$K$1</c:f>
@@ -5394,20 +5016,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AD24-4FB8-B210-037E9C2A0669}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50040001"/>
         <c:axId val="50040002"/>
@@ -5417,7 +5026,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5435,25 +5043,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50040002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50040002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5471,11 +5074,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50040001"/>
         <c:crosses val="autoZero"/>
@@ -5484,11 +5085,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5499,26 +5098,14 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5533,7 +5120,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Valencia vs R. Sociedad'!$B$1:$K$1</c:f>
@@ -5611,11 +5197,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-902F-46B7-987F-1962DD812BD9}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5631,7 +5212,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Valencia vs R. Sociedad'!$B$1:$K$1</c:f>
@@ -5709,20 +5289,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-902F-46B7-987F-1962DD812BD9}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50050001"/>
         <c:axId val="50050002"/>
@@ -5732,7 +5299,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5750,25 +5316,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50050002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50050002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5786,11 +5347,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50050001"/>
         <c:crosses val="autoZero"/>
@@ -5799,11 +5358,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5814,26 +5371,14 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5848,7 +5393,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Athletic vs Girona'!$B$1:$K$1</c:f>
@@ -5926,11 +5470,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D8E5-4D52-98CC-3FD9D959F5B7}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5946,7 +5485,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Athletic vs Girona'!$B$1:$K$1</c:f>
@@ -6024,20 +5562,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D8E5-4D52-98CC-3FD9D959F5B7}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50060001"/>
         <c:axId val="50060002"/>
@@ -6047,7 +5572,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -6065,25 +5589,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50060002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50060002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -6101,11 +5620,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50060001"/>
         <c:crosses val="autoZero"/>
@@ -6114,11 +5631,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -6129,26 +5644,14 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -6163,7 +5666,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Celta vs Real Valladolid'!$B$1:$K$1</c:f>
@@ -6241,11 +5743,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-64E5-4D5F-AB04-5C6083BA2B8D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -6261,7 +5758,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Celta vs Real Valladolid'!$B$1:$K$1</c:f>
@@ -6339,20 +5835,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-64E5-4D5F-AB04-5C6083BA2B8D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50070001"/>
         <c:axId val="50070002"/>
@@ -6362,7 +5845,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -6380,25 +5862,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50070002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50070002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -6416,11 +5893,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50070001"/>
         <c:crosses val="autoZero"/>
@@ -6429,11 +5904,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -6444,26 +5917,14 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -6478,7 +5939,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'AlmerÃ­a vs Barcelona'!$B$1:$K$1</c:f>
@@ -6556,11 +6016,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2A7F-458F-B9D6-BBCBC09052C1}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -6576,7 +6031,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'AlmerÃ­a vs Barcelona'!$B$1:$K$1</c:f>
@@ -6654,20 +6108,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2A7F-458F-B9D6-BBCBC09052C1}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50080001"/>
         <c:axId val="50080002"/>
@@ -6677,7 +6118,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -6695,25 +6135,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50080002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50080002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -6731,11 +6166,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50080001"/>
         <c:crosses val="autoZero"/>
@@ -6744,11 +6177,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -6759,26 +6190,14 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -6793,7 +6212,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Sevilla vs Osasuna'!$B$1:$K$1</c:f>
@@ -6871,11 +6289,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6366-4DE0-903B-6A958A127296}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -6891,7 +6304,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Sevilla vs Osasuna'!$B$1:$K$1</c:f>
@@ -6969,20 +6381,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6366-4DE0-903B-6A958A127296}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50090001"/>
         <c:axId val="50090002"/>
@@ -6992,7 +6391,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -7010,25 +6408,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50090002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50090002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -7046,11 +6439,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50090001"/>
         <c:crosses val="autoZero"/>
@@ -7059,11 +6450,9 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -7090,13 +6479,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7131,13 +6514,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7160,25 +6537,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1228725</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7213,13 +6584,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7247,20 +6612,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7295,13 +6654,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7336,13 +6689,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7377,13 +6724,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7418,13 +6759,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7459,13 +6794,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7500,13 +6829,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7525,7 +6848,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7567,7 +6890,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7599,27 +6922,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7651,24 +6956,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7844,17 +7131,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7889,7 +7176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7924,7 +7211,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -7966,17 +7253,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8011,7 +7298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -8046,7 +7333,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -8088,21 +7375,17 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:V46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="40.85546875" customWidth="1"/>
-    <col min="11" max="23" width="20.7109375" customWidth="1"/>
+    <col min="1" max="23" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -8170,7 +7453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -8238,7 +7521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -8306,7 +7589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -8374,7 +7657,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -8442,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -8510,7 +7793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -8578,7 +7861,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -8646,143 +7929,143 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:22">
+      <c r="A9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9">
         <v>6</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9">
         <v>6</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9">
         <v>4</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9">
         <v>0</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9">
         <v>2</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9">
         <v>0</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9">
         <v>1.2</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9">
         <v>1.2</v>
       </c>
-      <c r="U9" s="3">
+      <c r="U9">
         <v>32</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V9">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:22">
+      <c r="A10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" t="s">
         <v>93</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" t="s">
         <v>110</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" t="s">
         <v>94</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10">
         <v>4</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10">
         <v>9</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10">
         <v>2</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10">
         <v>0</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10">
         <v>4</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10">
         <v>0</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10">
         <v>0.8</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10">
         <v>1.8</v>
       </c>
-      <c r="U10" s="3">
+      <c r="U10">
         <v>18</v>
       </c>
-      <c r="V10" s="3">
+      <c r="V10">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -8850,7 +8133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -8918,7 +8201,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -8986,7 +8269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -9054,7 +8337,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -9122,7 +8405,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -9190,7 +8473,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -9258,7 +8541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -9326,7 +8609,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -9394,7 +8677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -9462,7 +8745,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -9527,237 +8810,6 @@
         <v>18</v>
       </c>
       <c r="V21">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>37</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28">
-        <v>20</v>
-      </c>
-      <c r="C28">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29">
-        <v>19</v>
-      </c>
-      <c r="C29">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30">
-        <v>33</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31">
-        <v>20</v>
-      </c>
-      <c r="C31">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32">
-        <v>19</v>
-      </c>
-      <c r="C32">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33">
-        <v>31</v>
-      </c>
-      <c r="C33">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34">
-        <v>32</v>
-      </c>
-      <c r="C34">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35">
-        <v>18</v>
-      </c>
-      <c r="C35">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37">
-        <v>19</v>
-      </c>
-      <c r="C37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38">
-        <v>32</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39">
-        <v>19</v>
-      </c>
-      <c r="C39">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40">
-        <v>31</v>
-      </c>
-      <c r="C40">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41">
-        <v>19</v>
-      </c>
-      <c r="C41">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43">
-        <v>18</v>
-      </c>
-      <c r="C43">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44">
-        <v>31</v>
-      </c>
-      <c r="C44">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46">
-        <v>18</v>
-      </c>
-      <c r="C46">
         <v>36</v>
       </c>
     </row>
@@ -9768,17 +8820,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9813,7 +8865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -9848,7 +8900,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9890,19 +8942,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9937,7 +8987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -9972,7 +9022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -10005,36 +9055,6 @@
       </c>
       <c r="K3">
         <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J14" t="s">
-        <v>129</v>
-      </c>
-      <c r="K14">
-        <v>59</v>
-      </c>
-      <c r="L14" s="2">
-        <f>K14/$K$16</f>
-        <v>1.7352941176470589</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J15" t="s">
-        <v>130</v>
-      </c>
-      <c r="K15">
-        <v>34</v>
-      </c>
-      <c r="L15">
-        <f>K15/$K$16</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K16">
-        <f>MIN(K14:K15)</f>
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -10044,17 +9064,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10089,7 +9109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -10124,7 +9144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -10166,17 +9186,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10211,7 +9231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -10246,7 +9266,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10288,17 +9308,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10333,7 +9353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -10368,7 +9388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -10410,17 +9430,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10455,7 +9475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -10490,7 +9510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -10532,17 +9552,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10577,7 +9597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -10612,7 +9632,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -10654,17 +9674,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10699,7 +9719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -10734,7 +9754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Arbitros implementado, falta mejora
</commit_message>
<xml_diff>
--- a/Output Primera Division.xlsx
+++ b/Output Primera Division.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\Desktop\Projects\Python Programs\Bets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B829553B-E424-48B0-B077-4DCA85ECD41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elche vs Real Betis" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
     <sheet name="Villarreal vs Getafe" sheetId="10" r:id="rId10"/>
     <sheet name="Data Raw Primera" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -416,8 +422,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,18 +486,38 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -506,6 +532,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Elche vs Real Betis'!$B$1:$K$1</c:f>
@@ -583,6 +610,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3A89-44BB-B1A8-FC535B103441}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -598,6 +630,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Elche vs Real Betis'!$B$1:$K$1</c:f>
@@ -675,7 +708,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3A89-44BB-B1A8-FC535B103441}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
@@ -685,6 +731,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -702,20 +749,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -733,9 +785,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
@@ -744,9 +798,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -757,14 +813,26 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -779,6 +847,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Villarreal vs Getafe'!$B$1:$K$1</c:f>
@@ -856,6 +925,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-285E-450F-B5C0-15A277814088}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -871,6 +945,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Villarreal vs Getafe'!$B$1:$K$1</c:f>
@@ -948,7 +1023,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-285E-450F-B5C0-15A277814088}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50100001"/>
         <c:axId val="50100002"/>
@@ -958,6 +1046,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -975,20 +1064,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50100002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50100002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1006,9 +1100,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50100001"/>
         <c:crosses val="autoZero"/>
@@ -1017,9 +1113,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1030,14 +1128,26 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1052,6 +1162,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1133,25 +1244,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1195,6 +1306,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1210,6 +1326,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1291,25 +1408,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1353,6 +1470,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1368,6 +1490,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1449,25 +1572,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1511,6 +1634,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1526,6 +1654,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1607,25 +1736,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1669,6 +1798,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1684,6 +1818,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1765,25 +1900,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1827,6 +1962,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1842,6 +1982,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -1923,25 +2064,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1985,6 +2126,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -2000,6 +2146,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2081,25 +2228,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2143,6 +2290,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -2158,6 +2310,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2239,25 +2392,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2301,6 +2454,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
@@ -2316,6 +2474,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2397,25 +2556,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2459,6 +2618,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
@@ -2474,6 +2638,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2555,25 +2720,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2617,6 +2782,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
@@ -2632,6 +2802,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2713,25 +2884,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2775,6 +2946,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
@@ -2790,6 +2966,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -2871,25 +3048,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2933,6 +3110,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="12"/>
@@ -2948,6 +3130,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3029,25 +3212,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3091,6 +3274,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="13"/>
@@ -3106,6 +3294,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3187,25 +3376,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3249,6 +3438,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="14"/>
@@ -3264,6 +3458,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3345,25 +3540,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3407,6 +3602,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="15"/>
@@ -3422,6 +3622,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3503,25 +3704,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3565,6 +3766,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="16"/>
@@ -3580,6 +3786,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3661,25 +3868,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3723,6 +3930,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="17"/>
@@ -3738,6 +3950,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3819,25 +4032,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3881,6 +4094,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="18"/>
@@ -3896,6 +4114,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -3977,25 +4196,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4039,6 +4258,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="19"/>
@@ -4054,6 +4278,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Raw Primera'!$B$1:$V$1</c:f>
@@ -4135,25 +4360,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4197,7 +4422,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-DE4D-4D25-AFDB-8C0C8E9FDDD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50110001"/>
         <c:axId val="50110002"/>
@@ -4207,6 +4445,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4224,20 +4463,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50110002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50110002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -4255,9 +4499,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50110001"/>
         <c:crosses val="autoZero"/>
@@ -4266,9 +4512,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4279,14 +4527,26 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4301,6 +4561,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Espanyol vs Mallorca'!$B$1:$K$1</c:f>
@@ -4378,6 +4639,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0991-4EF5-9DAC-70BB0E8D08F5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4393,6 +4659,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Espanyol vs Mallorca'!$B$1:$K$1</c:f>
@@ -4470,7 +4737,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0991-4EF5-9DAC-70BB0E8D08F5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50020001"/>
         <c:axId val="50020002"/>
@@ -4480,6 +4760,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4497,20 +4778,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50020002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -4528,9 +4814,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
@@ -4539,9 +4827,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4552,14 +4842,26 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4574,6 +4876,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'CÃ¡diz vs Rayo Vallecano'!$B$1:$K$1</c:f>
@@ -4651,6 +4954,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6DB9-4C35-903C-CE1E3B397D50}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4666,6 +4974,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'CÃ¡diz vs Rayo Vallecano'!$B$1:$K$1</c:f>
@@ -4743,7 +5052,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6DB9-4C35-903C-CE1E3B397D50}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50030001"/>
         <c:axId val="50030002"/>
@@ -4753,6 +5075,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4770,20 +5093,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50030002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -4801,9 +5129,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030001"/>
         <c:crosses val="autoZero"/>
@@ -4812,9 +5142,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4825,14 +5157,26 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4847,6 +5191,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Real Madrid vs AtlÃ©tico'!$B$1:$K$1</c:f>
@@ -4924,6 +5269,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BC83-4D19-8635-006600731E97}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4939,6 +5289,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Real Madrid vs AtlÃ©tico'!$B$1:$K$1</c:f>
@@ -5016,7 +5367,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BC83-4D19-8635-006600731E97}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50040001"/>
         <c:axId val="50040002"/>
@@ -5026,6 +5390,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5043,20 +5408,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50040002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50040002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5074,9 +5444,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50040001"/>
         <c:crosses val="autoZero"/>
@@ -5085,9 +5457,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5098,14 +5472,26 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5120,6 +5506,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Valencia vs R. Sociedad'!$B$1:$K$1</c:f>
@@ -5197,6 +5584,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C3F-4CFC-910B-51ABEEAB90A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5212,6 +5604,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Valencia vs R. Sociedad'!$B$1:$K$1</c:f>
@@ -5289,7 +5682,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8C3F-4CFC-910B-51ABEEAB90A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50050001"/>
         <c:axId val="50050002"/>
@@ -5299,6 +5705,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5316,20 +5723,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50050002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50050002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5347,9 +5759,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50050001"/>
         <c:crosses val="autoZero"/>
@@ -5358,9 +5772,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5371,14 +5787,26 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5393,6 +5821,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Athletic vs Girona'!$B$1:$K$1</c:f>
@@ -5470,6 +5899,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C1BB-4400-9147-76BC449E2D0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5485,6 +5919,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Athletic vs Girona'!$B$1:$K$1</c:f>
@@ -5562,7 +5997,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C1BB-4400-9147-76BC449E2D0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50060001"/>
         <c:axId val="50060002"/>
@@ -5572,6 +6020,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5589,20 +6038,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50060002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50060002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5620,9 +6074,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50060001"/>
         <c:crosses val="autoZero"/>
@@ -5631,9 +6087,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5644,14 +6102,26 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5666,6 +6136,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Celta vs Real Valladolid'!$B$1:$K$1</c:f>
@@ -5743,6 +6214,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6409-4DEC-A6CA-4877E203CB1C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5758,6 +6234,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Celta vs Real Valladolid'!$B$1:$K$1</c:f>
@@ -5835,7 +6312,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6409-4DEC-A6CA-4877E203CB1C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50070001"/>
         <c:axId val="50070002"/>
@@ -5845,6 +6335,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5862,20 +6353,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50070002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50070002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5893,9 +6389,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50070001"/>
         <c:crosses val="autoZero"/>
@@ -5904,9 +6402,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5917,14 +6417,26 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5939,6 +6451,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'AlmerÃ­a vs Barcelona'!$B$1:$K$1</c:f>
@@ -6016,6 +6529,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-090D-4BFD-95CA-808407CBD33D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -6031,6 +6549,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'AlmerÃ­a vs Barcelona'!$B$1:$K$1</c:f>
@@ -6108,7 +6627,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-090D-4BFD-95CA-808407CBD33D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50080001"/>
         <c:axId val="50080002"/>
@@ -6118,6 +6650,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -6135,20 +6668,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50080002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50080002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -6166,9 +6704,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50080001"/>
         <c:crosses val="autoZero"/>
@@ -6177,9 +6717,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -6190,14 +6732,26 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -6212,6 +6766,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Sevilla vs Osasuna'!$B$1:$K$1</c:f>
@@ -6289,6 +6844,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B883-44E5-A598-2B7494065F90}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -6304,6 +6864,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Sevilla vs Osasuna'!$B$1:$K$1</c:f>
@@ -6381,7 +6942,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B883-44E5-A598-2B7494065F90}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="300"/>
         <c:axId val="50090001"/>
         <c:axId val="50090002"/>
@@ -6391,6 +6965,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -6408,20 +6983,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50090002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50090002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -6439,9 +7019,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50090001"/>
         <c:crosses val="autoZero"/>
@@ -6450,9 +7032,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -6479,7 +7063,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6514,7 +7104,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6549,7 +7145,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6584,7 +7186,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6612,14 +7220,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6654,7 +7268,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6689,7 +7309,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6724,7 +7350,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6759,7 +7391,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6794,7 +7432,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6829,7 +7473,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6848,7 +7498,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6890,7 +7540,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6922,9 +7572,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6956,6 +7624,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7131,17 +7817,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7176,7 +7862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7211,7 +7897,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -7253,17 +7939,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7298,7 +7984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -7333,7 +8019,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -7375,17 +8061,17 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="23" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -7453,7 +8139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -7521,7 +8207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -7589,7 +8275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -7657,7 +8343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -7725,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -7793,7 +8479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -7861,7 +8547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -7929,7 +8615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -7997,7 +8683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -8065,7 +8751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -8133,7 +8819,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -8201,7 +8887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -8269,7 +8955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -8337,7 +9023,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -8405,7 +9091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -8473,7 +9159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -8541,7 +9227,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -8609,7 +9295,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -8677,7 +9363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -8745,7 +9431,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -8820,17 +9506,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8865,7 +9551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -8900,7 +9586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8942,17 +9628,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8987,7 +9675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -9022,7 +9710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -9064,17 +9752,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9109,7 +9797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -9144,7 +9832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -9186,17 +9874,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9231,7 +9919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -9266,7 +9954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9308,17 +9996,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9353,7 +10041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -9388,7 +10076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -9430,17 +10118,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9475,7 +10163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -9510,7 +10198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -9552,17 +10240,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9597,7 +10285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -9632,7 +10320,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -9674,17 +10362,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9719,7 +10407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -9754,7 +10442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>

</xml_diff>